<commit_message>
Added RunAppModelRun, with functionality for DerivedText within Widgets
</commit_message>
<xml_diff>
--- a/examples/notebooks/overheating/create_model_run.xlsx
+++ b/examples/notebooks/overheating/create_model_run.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
+  <si>
+    <t>Derived Value</t>
+  </si>
   <si>
     <t>Date Picker</t>
   </si>
@@ -118,7 +121,10 @@
     <t>Cooling: Technical Characteristics</t>
   </si>
   <si>
-    <t>12/06/2020</t>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>29/06/2020</t>
   </si>
   <si>
     <t>YY-OverheatingAnalysis</t>
@@ -506,7 +512,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -528,7 +534,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -538,8 +544,8 @@
       <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="C3">
-        <v>16</v>
+      <c r="C3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -549,8 +555,8 @@
       <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
-        <v>35</v>
+      <c r="C4">
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -560,6 +566,9 @@
       <c r="B5" t="s">
         <v>3</v>
       </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1">
@@ -568,9 +577,6 @@
       <c r="B6" t="s">
         <v>4</v>
       </c>
-      <c r="C6" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1">
@@ -591,7 +597,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -601,6 +607,9 @@
       <c r="B9" t="s">
         <v>7</v>
       </c>
+      <c r="C9" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1">
@@ -617,9 +626,6 @@
       <c r="B11" t="s">
         <v>9</v>
       </c>
-      <c r="C11" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1">
@@ -629,7 +635,7 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -639,6 +645,9 @@
       <c r="B13" t="s">
         <v>11</v>
       </c>
+      <c r="C13" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1">
@@ -647,9 +656,6 @@
       <c r="B14" t="s">
         <v>12</v>
       </c>
-      <c r="C14" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1">
@@ -658,8 +664,8 @@
       <c r="B15" t="s">
         <v>13</v>
       </c>
-      <c r="C15">
-        <v>55.1</v>
+      <c r="C15" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -670,7 +676,7 @@
         <v>14</v>
       </c>
       <c r="C16">
-        <v>0.1</v>
+        <v>55.1</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -714,7 +720,7 @@
         <v>18</v>
       </c>
       <c r="C20">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -725,7 +731,7 @@
         <v>19</v>
       </c>
       <c r="C21">
-        <v>0.9</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -736,7 +742,7 @@
         <v>20</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -747,7 +753,7 @@
         <v>21</v>
       </c>
       <c r="C23">
-        <v>0.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -758,7 +764,7 @@
         <v>22</v>
       </c>
       <c r="C24">
-        <v>3</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -768,8 +774,8 @@
       <c r="B25" t="s">
         <v>23</v>
       </c>
-      <c r="C25" t="s">
-        <v>39</v>
+      <c r="C25">
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -780,7 +786,7 @@
         <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -791,7 +797,7 @@
         <v>25</v>
       </c>
       <c r="C27" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -801,6 +807,9 @@
       <c r="B28" t="s">
         <v>26</v>
       </c>
+      <c r="C28" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="1">
@@ -809,16 +818,16 @@
       <c r="B29" t="s">
         <v>27</v>
       </c>
-      <c r="C29" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="1">
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>26</v>
+        <v>28</v>
+      </c>
+      <c r="C30" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -826,10 +835,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>28</v>
-      </c>
-      <c r="C31" t="b">
-        <v>1</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -850,8 +856,8 @@
       <c r="B33" t="s">
         <v>30</v>
       </c>
-      <c r="C33" t="s">
-        <v>42</v>
+      <c r="C33" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -862,7 +868,7 @@
         <v>31</v>
       </c>
       <c r="C34" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -873,7 +879,7 @@
         <v>32</v>
       </c>
       <c r="C35" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -884,7 +890,18 @@
         <v>33</v>
       </c>
       <c r="C36" t="s">
-        <v>43</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="1">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>34</v>
+      </c>
+      <c r="C37" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>